<commit_message>
size comparision from bytes to MB
</commit_message>
<xml_diff>
--- a/Metrics.xlsx
+++ b/Metrics.xlsx
@@ -25,7 +25,7 @@
     <t>Training Time in sec</t>
   </si>
   <si>
-    <t>Model size in bytes</t>
+    <t>Model size in Mega Bytes</t>
   </si>
   <si>
     <t>f score</t>
@@ -130,7 +130,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -481,7 +481,7 @@
         <v>65</v>
       </c>
       <c r="D2" s="6">
-        <v>1914319</v>
+        <v>1.914319</v>
       </c>
       <c r="E2" s="5">
         <v>0.99</v>
@@ -498,7 +498,7 @@
         <v>54000</v>
       </c>
       <c r="D3" s="6">
-        <v>985069</v>
+        <v>0.985069</v>
       </c>
       <c r="E3" s="5">
         <v>0.99</v>
@@ -515,7 +515,7 @@
         <v>0.2</v>
       </c>
       <c r="D4" s="6">
-        <v>7654996</v>
+        <v>7.654996</v>
       </c>
       <c r="E4" s="5">
         <v>0.98</v>
@@ -532,7 +532,7 @@
         <v>194.7</v>
       </c>
       <c r="D5" s="6">
-        <v>55423816</v>
+        <v>55.423816</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>9</v>
@@ -549,7 +549,7 @@
         <v>24</v>
       </c>
       <c r="D6" s="6">
-        <v>5197488</v>
+        <v>5.197488</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>9</v>
@@ -566,7 +566,7 @@
         <v>1022.01</v>
       </c>
       <c r="D7" s="6">
-        <v>123060035</v>
+        <v>123.060035</v>
       </c>
       <c r="E7" s="5">
         <v>0.97</v>
@@ -583,7 +583,7 @@
         <v>162.9</v>
       </c>
       <c r="D8" s="6">
-        <v>55220720</v>
+        <v>55.22072</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>9</v>

</xml_diff>